<commit_message>
The first spreadsheet I committed didn't show all of my paragraphs in the box
</commit_message>
<xml_diff>
--- a/Individual Systems Theory Assignment.xlsx
+++ b/Individual Systems Theory Assignment.xlsx
@@ -74,7 +74,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -82,6 +82,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -383,11 +386,14 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:D9"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>